<commit_message>
Step 3.5.4: Correction filtres - Filtrage côté serveur
- Ajout paramètres de filtre à transactionsAPI.getAll() et mappingsAPI.list()
- Passage des filtres texte (nom, level_1/2/3) à l'API dans MappingTable et TransactionsTable
- Suppression filtrage local pour MappingTable (API fait déjà le filtrage)
- Conservation filtrage local pour date, quantité, solde dans TransactionsTable (non supportés côté serveur)
- Réinitialisation page à 1 quand filtres changent
- Mise à jour IMPLEMENTATION_PLAN.md
</commit_message>
<xml_diff>
--- a/backend/data/input/trades/mapping copy 2.xlsx
+++ b/backend/data/input/trades/mapping copy 2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisgarnier/Library/Mobile Documents/com~apple~CloudDocs/Python/DEV/LMNP/scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisgarnier/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4382AC00-DEAC-3846-9432-C16EED6DFC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5024F8-6973-1544-92EC-C4EEC21282CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-11120" yWindow="-28300" windowWidth="30240" windowHeight="28060" xr2:uid="{C2A2B53B-49A6-234D-B395-58C1E4ECDF9F}"/>
   </bookViews>
@@ -370,18 +370,6 @@
     <t>pret banque - terrain</t>
   </si>
   <si>
-    <t>frais pr√™t</t>
-  </si>
-  <si>
-    <t>VIR PR√äT ACHAT APPART (construction)</t>
-  </si>
-  <si>
-    <t>VIR PR√äT ACHAT APPART (terrain)</t>
-  </si>
-  <si>
-    <t>pr√™t (inflows)</t>
-  </si>
-  <si>
     <t>VIR SEPA MASTEOS TRAVAUX n</t>
   </si>
   <si>
@@ -443,6 +431,18 @@
   </si>
   <si>
     <t>VIR STRIPE MANDA-IG8LSEBDSLSJUTIC5LQLEZJVCVXQJ MANDA</t>
+  </si>
+  <si>
+    <t>prêt (inflows)</t>
+  </si>
+  <si>
+    <t>VIR PRET ACHAT APPART (construction)</t>
+  </si>
+  <si>
+    <t>VIR PRET ACHAT APPART (terrain)</t>
+  </si>
+  <si>
+    <t>frais prêt</t>
   </si>
 </sst>
 </file>
@@ -797,7 +797,7 @@
   <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -975,7 +975,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="B13" t="s">
         <v>103</v>
@@ -1045,7 +1045,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="B18" t="s">
         <v>108</v>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="B19" t="s">
         <v>109</v>
@@ -1079,7 +1079,7 @@
         <v>101</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
@@ -1093,7 +1093,7 @@
         <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B26" t="s">
         <v>107</v>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B39" t="s">
         <v>20</v>
@@ -1353,7 +1353,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B40" t="s">
         <v>32</v>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B71" t="s">
         <v>37</v>
@@ -1801,7 +1801,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B72" t="s">
         <v>22</v>
@@ -1815,7 +1815,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B73" t="s">
         <v>20</v>
@@ -1829,7 +1829,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B74" t="s">
         <v>20</v>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B75" t="s">
         <v>37</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B76" t="s">
         <v>37</v>
@@ -1871,7 +1871,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B77" t="s">
         <v>105</v>
@@ -1885,7 +1885,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B78" t="s">
         <v>105</v>
@@ -1899,7 +1899,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B79" t="s">
         <v>71</v>
@@ -1913,7 +1913,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B80" t="s">
         <v>20</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B81" t="s">
         <v>20</v>
@@ -1941,7 +1941,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B82" t="s">
         <v>22</v>
@@ -1955,7 +1955,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B83" t="s">
         <v>37</v>
@@ -1969,7 +1969,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B84" t="s">
         <v>80</v>
@@ -1983,7 +1983,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B85" t="s">
         <v>80</v>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B86" t="s">
         <v>80</v>
@@ -2025,7 +2025,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B88" t="s">
         <v>80</v>
@@ -2039,7 +2039,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B89" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Step 4.1.1-4.1.5: Tableau croisé dynamique - Backend endpoints, API client, sélection champs, affichage tableau
- Step 4.1.1: Backend endpoint pivot (GET /api/analytics/pivot)
- Step 4.1.2: Backend endpoint details (GET /api/analytics/pivot/details)
- Step 4.1.3: Frontend API client (analyticsAPI)
- Step 4.1.4: Frontend panneau sélection champs (style Excel pin headers)
- Step 4.1.5: Frontend composant tableau croisé avec hiérarchie et expand/collapse

Fonctionnalités:
- Panneau latéral de configuration (hover/clic)
- Structure hiérarchique avec indentation (3+ niveaux)
- Expand/collapse des catégories
- Color code distinct par niveau (bleu/vert/violet/orange)
- Alternance zebra striping par niveau
- Totaux par niveau et grand total
- Clic sur cellules pour détails (préparé pour Step 4.1.6)
</commit_message>
<xml_diff>
--- a/backend/data/input/trades/mapping copy 2.xlsx
+++ b/backend/data/input/trades/mapping copy 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisgarnier/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5024F8-6973-1544-92EC-C4EEC21282CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A38780-59C6-0F47-B632-A89E3FB0140B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11120" yWindow="-28300" windowWidth="30240" windowHeight="28060" xr2:uid="{C2A2B53B-49A6-234D-B395-58C1E4ECDF9F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{C2A2B53B-49A6-234D-B395-58C1E4ECDF9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -373,12 +373,6 @@
     <t>VIR SEPA MASTEOS TRAVAUX n</t>
   </si>
   <si>
-    <t>Virement re‚àö√üu du 06/10/2022 (cash pour payer les charges)</t>
-  </si>
-  <si>
-    <t>Virement re‚àö√üu du 06/10/2022 (piement des charges)</t>
-  </si>
-  <si>
     <t>VIR STRIPE MANDA-ZNFQWZHWIWS1XCUOVYWOU2QFWHICZ MANDA</t>
   </si>
   <si>
@@ -443,6 +437,12 @@
   </si>
   <si>
     <t>frais prêt</t>
+  </si>
+  <si>
+    <t>Virement recu du 06/10/2022 (cash pour payer les charges)</t>
+  </si>
+  <si>
+    <t>Virement recu du 06/10/2022 (piement des charges)</t>
   </si>
 </sst>
 </file>
@@ -796,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27191FC7-05AA-4246-8E85-56E4F433B247}">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -975,7 +975,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
         <v>103</v>
@@ -1045,7 +1045,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
         <v>108</v>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B19" t="s">
         <v>109</v>
@@ -1079,7 +1079,7 @@
         <v>101</v>
       </c>
       <c r="C20" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
@@ -1093,7 +1093,7 @@
         <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="B39" t="s">
         <v>20</v>
@@ -1353,7 +1353,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="B40" t="s">
         <v>32</v>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B71" t="s">
         <v>37</v>
@@ -1801,7 +1801,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B72" t="s">
         <v>22</v>
@@ -1815,7 +1815,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B73" t="s">
         <v>20</v>
@@ -1829,7 +1829,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B74" t="s">
         <v>20</v>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B75" t="s">
         <v>37</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B76" t="s">
         <v>37</v>
@@ -1871,7 +1871,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B77" t="s">
         <v>105</v>
@@ -1885,7 +1885,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B78" t="s">
         <v>105</v>
@@ -1899,7 +1899,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B79" t="s">
         <v>71</v>
@@ -1913,7 +1913,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B80" t="s">
         <v>20</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B81" t="s">
         <v>20</v>
@@ -1941,7 +1941,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B82" t="s">
         <v>22</v>
@@ -1955,7 +1955,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B83" t="s">
         <v>37</v>
@@ -1969,7 +1969,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B84" t="s">
         <v>80</v>
@@ -1983,7 +1983,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B85" t="s">
         <v>80</v>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B86" t="s">
         <v>80</v>
@@ -2025,7 +2025,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B88" t="s">
         <v>80</v>
@@ -2039,7 +2039,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B89" t="s">
         <v>37</v>

</xml_diff>